<commit_message>
LogOutageDetection writes to CSV file. Attention: overwrites entries when executeLogOutageDetection() is started; writer should be declared and initialized in the main method.
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -12,9 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Technical Log Columnname</t>
+  </si>
+  <si>
+    <t>Log Event</t>
+  </si>
+  <si>
+    <t>Ausfallzeit</t>
+  </si>
+  <si>
+    <t>Wiederstartzeit</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Okay?</t>
+  </si>
+  <si>
+    <t>Grund</t>
+  </si>
   <si>
     <t>Hallo</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -59,16 +86,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.02734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="25.5234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.70703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.265625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.96875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.0" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.5625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>